<commit_message>
Operation Chaining 6ns vivado report aggiornati
</commit_message>
<xml_diff>
--- a/reports/vivado/OperationChaining6nsSolution/power/OperationChaining6nsClockEnablePowerReport.xlsx
+++ b/reports/vivado/OperationChaining6nsSolution/power/OperationChaining6nsClockEnablePowerReport.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>Utilization</t>
   </si>
@@ -44,19 +44,28 @@
     <t/>
   </si>
   <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state7</t>
+  </si>
+  <si>
+    <t>myclk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DSP FF LUT </t>
+  </si>
+  <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state13</t>
   </si>
   <si>
-    <t>myclk</t>
-  </si>
-  <si>
     <t xml:space="preserve">FF LUT </t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DSP FF LUT </t>
+    <t>firConvolutionOperationChaining_IP/U0/shiftRegister_U/firConvolutionOpebkb_ram_U/q0[31]_i_1_n_0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF </t>
+  </si>
+  <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state12</t>
   </si>
   <si>
     <t>firConvolutionOperationChaining_IP/U0/shiftRegister_U/firConvolutionOpebkb_ram_U/p_0_in_0</t>
@@ -65,58 +74,40 @@
     <t xml:space="preserve">RAM </t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/shiftRegister_U/firConvolutionOpebkb_ram_U/q0[31]_i_1_n_0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FF </t>
-  </si>
-  <si>
     <t>firConvolutionOperationChaining_IP/U0/p_pn_reg_118[31]_i_1_n_0</t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state12</t>
-  </si>
-  <si>
     <t>firConvolutionOperationChaining_IP/U0/ce0</t>
   </si>
   <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[8]</t>
+  </si>
+  <si>
     <t>firConvolutionOperationChaining_IP/U0/shiftRegister_U/firConvolutionOpebkb_ram_U/E[0]</t>
   </si>
   <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[10]</t>
+  </si>
+  <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[5]</t>
+  </si>
+  <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[7]</t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[8]</t>
-  </si>
-  <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[9]</t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[10]</t>
-  </si>
-  <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_state5</t>
   </si>
   <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[5]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[6]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[12]</t>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[2]</t>
+  </si>
+  <si>
+    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[3]</t>
   </si>
   <si>
     <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[1]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[2]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_CS_fsm_reg_n_0_[3]</t>
-  </si>
-  <si>
-    <t>firConvolutionOperationChaining_IP/U0/ap_NS_fsm[1]</t>
   </si>
 </sst>
 </file>
@@ -238,7 +229,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n" s="2">
-        <v>6.51370792184025E-4</v>
+        <v>3.6785000702366233E-4</v>
       </c>
       <c r="B2" t="s" s="4">
         <v>8</v>
@@ -264,22 +255,22 @@
     </row>
     <row r="3" outlineLevel="1">
       <c r="A3" t="n" s="5">
-        <v>1.9686520681716502E-4</v>
+        <v>1.0025110532296821E-4</v>
       </c>
       <c r="B3" t="s" s="4">
         <v>10</v>
       </c>
       <c r="C3" t="n" s="2">
-        <v>39.68254089355469</v>
+        <v>36.349205017089844</v>
       </c>
       <c r="D3" t="n" s="2">
-        <v>11.904762268066406</v>
+        <v>10.912285804748535</v>
       </c>
       <c r="E3" t="n" s="7">
-        <v>105.0</v>
+        <v>88.0</v>
       </c>
       <c r="F3" t="n" s="7">
-        <v>0.0</v>
+        <v>28.0</v>
       </c>
       <c r="G3" t="s" s="4">
         <v>11</v>
@@ -290,22 +281,22 @@
     </row>
     <row r="4" outlineLevel="1">
       <c r="A4" t="n" s="5">
-        <v>1.4119049592409283E-4</v>
+        <v>9.444444731343538E-5</v>
       </c>
       <c r="B4" t="s" s="4">
         <v>13</v>
       </c>
       <c r="C4" t="n" s="2">
-        <v>36.349205017089844</v>
+        <v>39.68254089355469</v>
       </c>
       <c r="D4" t="n" s="2">
-        <v>10.912285804748535</v>
+        <v>11.904762268066406</v>
       </c>
       <c r="E4" t="n" s="7">
-        <v>88.0</v>
+        <v>105.0</v>
       </c>
       <c r="F4" t="n" s="7">
-        <v>0.0</v>
+        <v>21.0</v>
       </c>
       <c r="G4" t="s" s="4">
         <v>11</v>
@@ -316,7 +307,7 @@
     </row>
     <row r="5" outlineLevel="1">
       <c r="A5" t="n" s="5">
-        <v>5.505872468347661E-5</v>
+        <v>3.508024019538425E-5</v>
       </c>
       <c r="B5" t="s" s="4">
         <v>15</v>
@@ -325,13 +316,13 @@
         <v>39.841270446777344</v>
       </c>
       <c r="D5" t="n" s="2">
-        <v>11.934745788574219</v>
+        <v>21.577285766601562</v>
       </c>
       <c r="E5" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F5" t="n" s="7">
-        <v>0.0</v>
+        <v>14.0</v>
       </c>
       <c r="G5" t="s" s="4">
         <v>11</v>
@@ -342,85 +333,85 @@
     </row>
     <row r="6" outlineLevel="1">
       <c r="A6" t="n" s="5">
-        <v>5.505872468347661E-5</v>
+        <v>2.7975236662314273E-5</v>
       </c>
       <c r="B6" t="s" s="4">
         <v>17</v>
       </c>
       <c r="C6" t="n" s="2">
-        <v>39.841270446777344</v>
+        <v>36.19047546386719</v>
       </c>
       <c r="D6" t="n" s="2">
-        <v>21.577285766601562</v>
+        <v>10.85714340209961</v>
       </c>
       <c r="E6" t="n" s="7">
-        <v>32.0</v>
+        <v>34.0</v>
       </c>
       <c r="F6" t="n" s="7">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="G6" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H6" t="s" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" outlineLevel="1">
       <c r="A7" t="n" s="5">
-        <v>5.483936911332421E-5</v>
+        <v>2.6315159630030394E-5</v>
       </c>
       <c r="B7" t="s" s="4">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C7" t="n" s="2">
-        <v>39.68254089355469</v>
+        <v>39.841270446777344</v>
       </c>
       <c r="D7" t="n" s="2">
-        <v>11.904762268066406</v>
+        <v>11.934745788574219</v>
       </c>
       <c r="E7" t="n" s="7">
         <v>32.0</v>
       </c>
       <c r="F7" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G7" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H7" t="s" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" outlineLevel="1">
       <c r="A8" t="n" s="5">
-        <v>5.025662903790362E-5</v>
+        <v>2.261904774059076E-5</v>
       </c>
       <c r="B8" t="s" s="4">
         <v>20</v>
       </c>
       <c r="C8" t="n" s="2">
-        <v>36.19047546386719</v>
+        <v>39.68254089355469</v>
       </c>
       <c r="D8" t="n" s="2">
-        <v>10.85714340209961</v>
+        <v>11.904762268066406</v>
       </c>
       <c r="E8" t="n" s="7">
-        <v>34.0</v>
+        <v>32.0</v>
       </c>
       <c r="F8" t="n" s="7">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="G8" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H8" t="s" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" outlineLevel="1">
       <c r="A9" t="n" s="5">
-        <v>4.710662688012235E-5</v>
+        <v>2.1919999198871665E-5</v>
       </c>
       <c r="B9" t="s" s="4">
         <v>21</v>
@@ -435,70 +426,70 @@
         <v>17.0</v>
       </c>
       <c r="F9" t="n" s="7">
-        <v>0.0</v>
+        <v>8.0</v>
       </c>
       <c r="G9" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H9" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" outlineLevel="1">
       <c r="A10" t="n" s="5">
-        <v>1.0047441719507333E-5</v>
+        <v>9.337142728327308E-6</v>
       </c>
       <c r="B10" t="s" s="4">
         <v>22</v>
       </c>
       <c r="C10" t="n" s="2">
-        <v>36.507938385009766</v>
+        <v>36.19047546386719</v>
       </c>
       <c r="D10" t="n" s="2">
-        <v>10.952381134033203</v>
+        <v>10.85714340209961</v>
       </c>
       <c r="E10" t="n" s="7">
-        <v>5.0</v>
+        <v>2.0</v>
       </c>
       <c r="F10" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G10" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H10" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" outlineLevel="1">
       <c r="A11" t="n" s="5">
-        <v>6.289943030424183E-6</v>
+        <v>6.589682925550733E-6</v>
       </c>
       <c r="B11" t="s" s="4">
         <v>23</v>
       </c>
       <c r="C11" t="n" s="2">
-        <v>36.19047546386719</v>
+        <v>36.507938385009766</v>
       </c>
       <c r="D11" t="n" s="2">
-        <v>10.85714340209961</v>
+        <v>10.952381134033203</v>
       </c>
       <c r="E11" t="n" s="7">
-        <v>2.0</v>
+        <v>5.0</v>
       </c>
       <c r="F11" t="n" s="7">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="G11" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H11" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" outlineLevel="1">
       <c r="A12" t="n" s="5">
-        <v>6.289943030424183E-6</v>
+        <v>4.921904746879591E-6</v>
       </c>
       <c r="B12" t="s" s="4">
         <v>24</v>
@@ -513,44 +504,44 @@
         <v>2.0</v>
       </c>
       <c r="F12" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G12" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H12" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" outlineLevel="1">
       <c r="A13" t="n" s="5">
-        <v>6.289943030424183E-6</v>
+        <v>4.849364813708235E-6</v>
       </c>
       <c r="B13" t="s" s="4">
         <v>25</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>36.19047546386719</v>
+        <v>43.4920654296875</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>10.85714340209961</v>
+        <v>13.047618865966797</v>
       </c>
       <c r="E13" t="n" s="7">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="F13" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G13" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H13" t="s" s="4">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" outlineLevel="1">
       <c r="A14" t="n" s="5">
-        <v>6.289943030424183E-6</v>
+        <v>4.704761977336602E-6</v>
       </c>
       <c r="B14" t="s" s="4">
         <v>26</v>
@@ -565,122 +556,122 @@
         <v>2.0</v>
       </c>
       <c r="F14" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G14" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H14" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" outlineLevel="1">
       <c r="A15" t="n" s="5">
-        <v>5.3561902859655675E-6</v>
+        <v>4.704761977336602E-6</v>
       </c>
       <c r="B15" t="s" s="4">
         <v>27</v>
       </c>
       <c r="C15" t="n" s="2">
-        <v>3.8095240592956543</v>
+        <v>36.19047546386719</v>
       </c>
       <c r="D15" t="n" s="2">
-        <v>1.1428569555282593</v>
+        <v>10.85714340209961</v>
       </c>
       <c r="E15" t="n" s="7">
-        <v>35.0</v>
+        <v>2.0</v>
       </c>
       <c r="F15" t="n" s="7">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G15" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H15" t="s" s="4">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" outlineLevel="1">
       <c r="A16" t="n" s="5">
-        <v>2.892522161346278E-6</v>
+        <v>2.6628572413756046E-6</v>
       </c>
       <c r="B16" t="s" s="4">
         <v>28</v>
       </c>
       <c r="C16" t="n" s="2">
-        <v>43.4920654296875</v>
+        <v>3.8095240592956543</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>13.047618865966797</v>
+        <v>1.1428569555282593</v>
       </c>
       <c r="E16" t="n" s="7">
-        <v>1.0</v>
+        <v>35.0</v>
       </c>
       <c r="F16" t="n" s="7">
-        <v>0.0</v>
+        <v>9.0</v>
       </c>
       <c r="G16" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H16" t="s" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" outlineLevel="1">
       <c r="A17" t="n" s="5">
-        <v>2.6602758680382976E-6</v>
+        <v>7.276190672200755E-7</v>
       </c>
       <c r="B17" t="s" s="4">
         <v>29</v>
       </c>
       <c r="C17" t="n" s="2">
-        <v>40.0</v>
+        <v>3.8095240592956543</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>10.95036506652832</v>
+        <v>1.1428569555282593</v>
       </c>
       <c r="E17" t="n" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F17" t="n" s="7">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G17" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H17" t="s" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" outlineLevel="1">
       <c r="A18" t="n" s="5">
-        <v>2.6391626306576654E-6</v>
+        <v>3.7904763416918286E-7</v>
       </c>
       <c r="B18" t="s" s="4">
         <v>30</v>
       </c>
       <c r="C18" t="n" s="2">
-        <v>39.68254089355469</v>
+        <v>3.8095240592956543</v>
       </c>
       <c r="D18" t="n" s="2">
-        <v>11.644952774047852</v>
+        <v>1.1428569555282593</v>
       </c>
       <c r="E18" t="n" s="7">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F18" t="n" s="7">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G18" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H18" t="s" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" outlineLevel="1">
       <c r="A19" t="n" s="5">
-        <v>6.620992394346104E-7</v>
+        <v>3.6761903743354196E-7</v>
       </c>
       <c r="B19" t="s" s="4">
         <v>31</v>
@@ -695,91 +686,13 @@
         <v>2.0</v>
       </c>
       <c r="F19" t="n" s="7">
-        <v>0.0</v>
+        <v>2.0</v>
       </c>
       <c r="G19" t="s" s="4">
         <v>11</v>
       </c>
       <c r="H19" t="s" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" outlineLevel="1">
-      <c r="A20" t="n" s="5">
-        <v>6.620992394346104E-7</v>
-      </c>
-      <c r="B20" t="s" s="4">
-        <v>32</v>
-      </c>
-      <c r="C20" t="n" s="2">
-        <v>3.8095240592956543</v>
-      </c>
-      <c r="D20" t="n" s="2">
-        <v>1.1428569555282593</v>
-      </c>
-      <c r="E20" t="n" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="F20" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G20" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H20" t="s" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" outlineLevel="1">
-      <c r="A21" t="n" s="5">
-        <v>6.620992394346104E-7</v>
-      </c>
-      <c r="B21" t="s" s="4">
-        <v>33</v>
-      </c>
-      <c r="C21" t="n" s="2">
-        <v>3.8095240592956543</v>
-      </c>
-      <c r="D21" t="n" s="2">
-        <v>1.1428569555282593</v>
-      </c>
-      <c r="E21" t="n" s="7">
-        <v>2.0</v>
-      </c>
-      <c r="F21" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G21" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H21" t="s" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="22" outlineLevel="1">
-      <c r="A22" t="n" s="5">
-        <v>2.53359615953741E-7</v>
-      </c>
-      <c r="B22" t="s" s="4">
-        <v>34</v>
-      </c>
-      <c r="C22" t="n" s="2">
-        <v>3.8095240592956543</v>
-      </c>
-      <c r="D22" t="n" s="2">
-        <v>0.9980480074882507</v>
-      </c>
-      <c r="E22" t="n" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="F22" t="n" s="7">
-        <v>0.0</v>
-      </c>
-      <c r="G22" t="s" s="4">
-        <v>11</v>
-      </c>
-      <c r="H22" t="s" s="4">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>